<commit_message>
restored excel file with sample data
</commit_message>
<xml_diff>
--- a/SampleData/SunnyPortalExport20170820.xlsx
+++ b/SampleData/SunnyPortalExport20170820.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="25">
   <si>
     <t>SUNNY-MAIL</t>
   </si>
@@ -483,10 +483,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K26"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="G33" sqref="G33"/>
+      <selection activeCell="J43" sqref="J43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -742,7 +742,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:11">
+    <row r="17" spans="1:7">
       <c r="A17" t="s">
         <v>14</v>
       </c>
@@ -759,221 +759,6 @@
         <v>533</v>
       </c>
       <c r="G17">
-        <v>533</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11">
-      <c r="A20" t="s">
-        <v>10</v>
-      </c>
-      <c r="B20" t="s">
-        <v>14</v>
-      </c>
-      <c r="C20" t="s">
-        <v>14</v>
-      </c>
-      <c r="D20" t="s">
-        <v>14</v>
-      </c>
-      <c r="E20" t="s">
-        <v>14</v>
-      </c>
-      <c r="F20" t="s">
-        <v>14</v>
-      </c>
-      <c r="G20" t="s">
-        <v>14</v>
-      </c>
-      <c r="H20" t="s">
-        <v>14</v>
-      </c>
-      <c r="I20" t="s">
-        <v>14</v>
-      </c>
-      <c r="J20" t="s">
-        <v>14</v>
-      </c>
-      <c r="K20" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11">
-      <c r="A21" t="s">
-        <v>11</v>
-      </c>
-      <c r="B21">
-        <v>2000814023</v>
-      </c>
-      <c r="C21">
-        <v>2000814023</v>
-      </c>
-      <c r="D21">
-        <v>2000814023</v>
-      </c>
-      <c r="E21">
-        <v>2000814023</v>
-      </c>
-      <c r="F21">
-        <v>2000814023</v>
-      </c>
-      <c r="G21">
-        <v>2000814023</v>
-      </c>
-      <c r="H21">
-        <v>2000814023</v>
-      </c>
-      <c r="I21">
-        <v>2000814023</v>
-      </c>
-      <c r="J21">
-        <v>2000814023</v>
-      </c>
-      <c r="K21">
-        <v>2000814023</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11">
-      <c r="A22" t="s">
-        <v>12</v>
-      </c>
-      <c r="B22" t="s">
-        <v>15</v>
-      </c>
-      <c r="C22" t="s">
-        <v>16</v>
-      </c>
-      <c r="D22" t="s">
-        <v>17</v>
-      </c>
-      <c r="E22" t="s">
-        <v>18</v>
-      </c>
-      <c r="F22" t="s">
-        <v>19</v>
-      </c>
-      <c r="G22" t="s">
-        <v>20</v>
-      </c>
-      <c r="H22" t="s">
-        <v>21</v>
-      </c>
-      <c r="I22" t="s">
-        <v>22</v>
-      </c>
-      <c r="J22" t="s">
-        <v>23</v>
-      </c>
-      <c r="K22" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11">
-      <c r="A23" t="s">
-        <v>6</v>
-      </c>
-      <c r="B23" t="s">
-        <v>7</v>
-      </c>
-      <c r="C23" t="s">
-        <v>7</v>
-      </c>
-      <c r="D23" t="s">
-        <v>7</v>
-      </c>
-      <c r="E23" t="s">
-        <v>7</v>
-      </c>
-      <c r="F23" t="s">
-        <v>7</v>
-      </c>
-      <c r="G23" t="s">
-        <v>7</v>
-      </c>
-      <c r="H23" t="s">
-        <v>7</v>
-      </c>
-      <c r="I23" t="s">
-        <v>7</v>
-      </c>
-      <c r="J23" t="s">
-        <v>7</v>
-      </c>
-      <c r="K23" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11">
-      <c r="A24" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11">
-      <c r="A25">
-        <v>0.44937500000000002</v>
-      </c>
-      <c r="B25">
-        <v>27025</v>
-      </c>
-      <c r="C25">
-        <v>29904</v>
-      </c>
-      <c r="D25">
-        <v>33358</v>
-      </c>
-      <c r="E25">
-        <v>3932</v>
-      </c>
-      <c r="F25">
-        <v>380</v>
-      </c>
-      <c r="G25">
-        <v>2000814023</v>
-      </c>
-      <c r="H25">
-        <v>1191</v>
-      </c>
-      <c r="I25">
-        <v>5</v>
-      </c>
-      <c r="J25">
-        <v>3</v>
-      </c>
-      <c r="K25">
-        <v>533</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11">
-      <c r="A26">
-        <v>0.45979166666666665</v>
-      </c>
-      <c r="B26">
-        <v>27025</v>
-      </c>
-      <c r="C26">
-        <v>29904</v>
-      </c>
-      <c r="D26">
-        <v>33358</v>
-      </c>
-      <c r="E26">
-        <v>3932</v>
-      </c>
-      <c r="F26">
-        <v>380</v>
-      </c>
-      <c r="G26">
-        <v>2000814023</v>
-      </c>
-      <c r="H26">
-        <v>941</v>
-      </c>
-      <c r="I26">
-        <v>4</v>
-      </c>
-      <c r="J26">
-        <v>3</v>
-      </c>
-      <c r="K26">
         <v>533</v>
       </c>
     </row>

</xml_diff>